<commit_message>
Added 2 more tests, Listeners, Status column, added waits, BeforeTest
</commit_message>
<xml_diff>
--- a/qbe/src/test/java/resources/QBETests.xlsx
+++ b/qbe/src/test/java/resources/QBETests.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView windowHeight="12648" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
+  <definedNames>
+    <definedName name="status">Sheet1!$AI$2:$AI$8</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="70">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -217,12 +220,25 @@
   </si>
   <si>
     <t>Changes to the chassis of the vehicle,Higher engine performance than standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -301,34 +317,49 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -345,10 +376,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -383,7 +414,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -418,7 +449,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -512,21 +543,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -543,7 +574,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -595,29 +626,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" topLeftCell="Y2" workbookViewId="0">
+      <selection activeCell="AI8" sqref="AI8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="3"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="35" max="35" width="8.88671875" style="3"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="2" max="2" style="3" width="8.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="35" max="35" style="3" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="72" r="1" s="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -724,7 +755,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="144" r="2" s="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -812,9 +843,11 @@
       <c r="AH2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AI2" s="2"/>
+      <c r="AI2" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="3" spans="1:35" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row customFormat="1" ht="43.2" r="3" s="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -833,9 +866,11 @@
       <c r="F3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AI3" s="2"/>
+      <c r="AI3" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="4" spans="1:35" ht="86.4" x14ac:dyDescent="0.3">
+    <row ht="86.4" r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>60</v>
       </c>
@@ -848,6 +883,8 @@
       <c r="D4" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1">
         <v>2016</v>
       </c>
@@ -875,15 +912,18 @@
       <c r="O4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="Q4" s="1"/>
       <c r="R4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T4" t="s">
+      <c r="S4" s="1"/>
+      <c r="T4" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="U4" s="1"/>
       <c r="V4" s="1" t="s">
         <v>53</v>
       </c>
@@ -893,10 +933,12 @@
       <c r="X4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AA4">
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1">
         <v>2016</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AB4" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AC4" s="1" t="s">
@@ -917,13 +959,49 @@
       <c r="AH4" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="AI4" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AI5" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AI6" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AI7" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AI8" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AI9" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="AI2:AI8">
+    <cfRule dxfId="1" priority="2" type="expression">
+      <formula>AI2="Passed"</formula>
+    </cfRule>
+    <cfRule dxfId="0" priority="1" type="expression">
+      <formula>AI2="Failed"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="AG2" r:id="rId1"/>
-    <hyperlink ref="AG4" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="AG2"/>
+    <hyperlink r:id="rId2" ref="AG4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added feature to input test data using test case name
</commit_message>
<xml_diff>
--- a/qbe/src/test/java/resources/QBETests.xlsx
+++ b/qbe/src/test/java/resources/QBETests.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView windowHeight="12648" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="status">Sheet1!$AI$2:$AI$8</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -129,12 +129,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>TC_01</t>
-  </si>
-  <si>
-    <t>TC_02</t>
-  </si>
-  <si>
     <t>29/07/2018</t>
   </si>
   <si>
@@ -204,9 +198,6 @@
     <t>ABC123</t>
   </si>
   <si>
-    <t>TC_03</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
@@ -231,14 +222,25 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>Failed</t>
+    <t>form_fill_total</t>
+  </si>
+  <si>
+    <t>form_incorrect_rego</t>
+  </si>
+  <si>
+    <t>form_incorrect_cover_start_date</t>
+  </si>
+  <si>
+    <t>form_car_cost_too_low</t>
+  </si>
+  <si>
+    <t>Changes to the chassis of the vehicle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -317,31 +319,31 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -359,7 +361,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -376,10 +378,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -414,7 +416,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -449,7 +451,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -543,21 +545,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -574,7 +576,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -626,29 +628,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y2" workbookViewId="0">
-      <selection activeCell="AI8" sqref="AI8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="2" max="2" style="3" width="8.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="35" max="35" style="3" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="28.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.88671875" style="3" collapsed="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="8.88671875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="72" r="1" s="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -755,133 +757,133 @@
         <v>34</v>
       </c>
     </row>
-    <row customFormat="1" ht="144" r="2" s="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1">
         <v>2016</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="K2" s="1">
         <v>1798</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="Y2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Z2" s="1">
         <v>420</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AE2" s="1">
         <v>300</v>
       </c>
       <c r="AF2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AI2" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AH2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row customFormat="1" ht="43.2" r="3" s="1" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row ht="86.4" r="4" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -889,49 +891,49 @@
         <v>2016</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="K4" s="1">
         <v>1798</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="N4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S4" s="1"/>
       <c r="T4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U4" s="1"/>
       <c r="V4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
@@ -939,69 +941,141 @@
         <v>2016</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AE4" s="1">
         <v>300</v>
       </c>
       <c r="AF4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AG4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="AI4" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
+        <v>2016</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1798</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>420</v>
+      </c>
       <c r="AI5" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AI6" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AI7" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AI8" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="AI9" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="AI2:AI8">
-    <cfRule dxfId="1" priority="2" type="expression">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AI2="Passed"</formula>
     </cfRule>
-    <cfRule dxfId="0" priority="1" type="expression">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AI2="Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="AG2"/>
-    <hyperlink r:id="rId2" ref="AG4"/>
+    <hyperlink ref="AG2" r:id="rId1"/>
+    <hyperlink ref="AG4" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bad Code - ability to scroll and test if elements visible in viewport
</commit_message>
<xml_diff>
--- a/qbe/src/test/java/resources/QBETests.xlsx
+++ b/qbe/src/test/java/resources/QBETests.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -216,25 +216,34 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>form_fill_total</t>
+  </si>
+  <si>
+    <t>form_incorrect_rego</t>
+  </si>
+  <si>
+    <t>form_incorrect_cover_start_date</t>
+  </si>
+  <si>
+    <t>form_car_cost_too_low</t>
+  </si>
+  <si>
+    <t>Changes to the chassis of the vehicle</t>
+  </si>
+  <si>
+    <t>form_scrolling</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>form_fill_total</t>
-  </si>
-  <si>
-    <t>form_incorrect_rego</t>
-  </si>
-  <si>
-    <t>form_incorrect_cover_start_date</t>
-  </si>
-  <si>
-    <t>form_car_cost_too_low</t>
-  </si>
-  <si>
-    <t>Changes to the chassis of the vehicle</t>
+    <t>form_submitted_with_empty_fields</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -638,13 +647,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="X2" workbookViewId="0">
+      <selection activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="8.88671875" style="3" collapsed="1"/>
     <col min="4" max="4" width="19.5546875" customWidth="1" collapsed="1"/>
     <col min="35" max="35" width="8.88671875" style="3" collapsed="1"/>
@@ -759,7 +768,7 @@
     </row>
     <row r="2" spans="1:35" s="1" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>35</v>
@@ -846,12 +855,12 @@
         <v>57</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:35" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>35</v>
@@ -869,12 +878,12 @@
         <v>39</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>35</v>
@@ -961,13 +970,13 @@
       <c r="AH4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AI4" s="1" t="s">
-        <v>65</v>
+      <c r="AI4" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>35</v>
@@ -1021,7 +1030,7 @@
         <v>49</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>51</v>
@@ -1036,20 +1045,52 @@
         <v>49</v>
       </c>
       <c r="Z5" s="1">
-        <v>420</v>
+        <v>9.01</v>
       </c>
       <c r="AI5" s="3" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
       <c r="AI6" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
+        <v>2016</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1798</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="AI7" s="3" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
All pass tests in suite
</commit_message>
<xml_diff>
--- a/qbe/src/test/java/resources/QBETests.xlsx
+++ b/qbe/src/test/java/resources/QBETests.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="73">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -877,7 +877,7 @@
         <v>39</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row ht="86.4" r="4" spans="1:35" x14ac:dyDescent="0.3">
@@ -970,7 +970,7 @@
         <v>57</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row ht="86.4" r="5" spans="1:35" x14ac:dyDescent="0.3">
@@ -1047,7 +1047,7 @@
         <v>9</v>
       </c>
       <c r="AI5" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
@@ -1055,7 +1055,7 @@
         <v>68</v>
       </c>
       <c r="AI6" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row ht="86.4" r="7" spans="1:35" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added browser as a command option
</commit_message>
<xml_diff>
--- a/qbe/src/test/java/resources/QBETests.xlsx
+++ b/qbe/src/test/java/resources/QBETests.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="73">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -854,7 +854,7 @@
         <v>57</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row customFormat="1" ht="43.2" r="3" s="1" spans="1:35" x14ac:dyDescent="0.3">
@@ -877,7 +877,7 @@
         <v>39</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row ht="86.4" r="4" spans="1:35" x14ac:dyDescent="0.3">
@@ -970,7 +970,7 @@
         <v>57</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row ht="86.4" r="5" spans="1:35" x14ac:dyDescent="0.3">
@@ -1047,7 +1047,7 @@
         <v>9</v>
       </c>
       <c r="AI5" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.3">
@@ -1055,7 +1055,7 @@
         <v>68</v>
       </c>
       <c r="AI6" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row ht="86.4" r="7" spans="1:35" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added HTMLUnit & PhantomJS, and Screenshot Listener features
</commit_message>
<xml_diff>
--- a/qbe/src/test/java/resources/QBETests.xlsx
+++ b/qbe/src/test/java/resources/QBETests.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="73">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -854,7 +854,7 @@
         <v>57</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row customFormat="1" ht="43.2" r="3" s="1" spans="1:35" x14ac:dyDescent="0.3">
@@ -877,7 +877,7 @@
         <v>39</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row ht="86.4" r="4" spans="1:35" x14ac:dyDescent="0.3">

</xml_diff>